<commit_message>
find mostly cited sutta
</commit_message>
<xml_diff>
--- a/paranum.xlsx
+++ b/paranum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20730" windowHeight="8145"/>
+    <workbookView windowWidth="20490" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="209">
   <si>
     <t>assuming on range (the last one) is addressable</t>
   </si>
@@ -235,6 +235,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>s0401t(1032) ,1-19,</t>
     </r>
     <r>
@@ -283,6 +290,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>t31s0403t1(459) ,1-196,1-16</t>
     </r>
     <r>
@@ -836,6 +850,9 @@
     <t>a53e0104n(1819) ,^365-892</t>
   </si>
   <si>
+    <t>abh04t anutika 法集</t>
+  </si>
+  <si>
     <t>abh01m(2435) ,1-22,1-142,1-1616</t>
   </si>
   <si>
@@ -845,7 +862,7 @@
     <t>abh01t(709) ,1-20,1-22,1-142,1-1577</t>
   </si>
   <si>
-    <t>abh04t anutika 法集</t>
+    <t>t41abh04t(721) ,1-17,1-22,1-142,1-1577</t>
   </si>
   <si>
     <t>abh02m(3419) ,1-1044</t>
@@ -999,7 +1016,7 @@
 1-23,1-21,1-45,1-56,1-28,1-66</t>
   </si>
   <si>
-    <t>t41abh04t(721) ,1-17,1-22,1-142,1-1577
+    <t xml:space="preserve">
 t42abh05t(1501) ,1-456,1-7,1-209,1-918,1-97,^2-208,1-254,1,^10-170,1-37,1-340,1-116,1-100,1-482,1-650,1-87,1-52,^51-72,^22-49
 t43abh06t(5398) ,1-1416,1-1857,1-1144,1-387
 t44abh07t(1575) ,1-43,1-60,1-74,1-55,1-102,1-65,1-53,1-43,1-75,1-43,1-60,1-74,1-55,1-102,1-65,1-53,1-43,1-75
@@ -1057,13 +1074,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1071,7 +1081,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1079,7 +1089,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1108,37 +1125,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1156,10 +1142,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1170,11 +1156,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1187,14 +1203,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1263,31 +1280,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1299,7 +1412,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1311,127 +1442,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1445,13 +1462,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1461,15 +1482,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1504,6 +1516,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1519,21 +1540,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1542,157 +1548,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1771,11 +1788,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2101,8 +2121,8 @@
   <sheetPr/>
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B16" sqref="B14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2675,16 +2695,16 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="21" t="s">
         <v>148</v>
       </c>
       <c r="E59" t="s">
@@ -2712,210 +2732,209 @@
         <v>154</v>
       </c>
     </row>
+    <row r="63" spans="4:4">
+      <c r="D63" t="s">
+        <v>155</v>
+      </c>
+    </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B64" s="3" t="s">
+      <c r="A64" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="B64" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C64" s="21" t="s">
         <v>158</v>
+      </c>
+      <c r="D64" s="21" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D65" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" ht="30" spans="1:5">
       <c r="A67" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E67" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B68" s="10" t="s">
+      <c r="A68" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="B68" s="26" t="s">
         <v>171</v>
       </c>
+      <c r="C68" s="26" t="s">
+        <v>172</v>
+      </c>
       <c r="D68" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" ht="22" customHeight="1" spans="1:4">
       <c r="A69" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D69" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B70" s="8" t="s">
+      <c r="A70" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="B70" s="28" t="s">
         <v>179</v>
       </c>
+      <c r="C70" s="28" t="s">
+        <v>180</v>
+      </c>
       <c r="D70" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="71" ht="30" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B71" s="26" t="s">
+      <c r="A71" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="B71" s="24" t="s">
         <v>183</v>
       </c>
+      <c r="C71" s="28" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B72" s="8" t="s">
+      <c r="A72" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="B72" s="28" t="s">
         <v>186</v>
       </c>
+      <c r="C72" s="28" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B73" s="8" t="s">
+      <c r="A73" s="27" t="s">
         <v>188</v>
       </c>
-      <c r="C73" s="8" t="s">
-        <v>188</v>
+      <c r="B73" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C73" s="28" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="74" customHeight="1" spans="1:3">
-      <c r="A74" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B74" s="8" t="s">
+      <c r="A74" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="C74" s="8" t="s">
+      <c r="B74" s="28" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="75" ht="43" customHeight="1" spans="1:4">
-      <c r="A75" s="27" t="s">
+      <c r="C74" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="B75" s="26" t="s">
+    </row>
+    <row r="75" ht="43" customHeight="1" spans="1:3">
+      <c r="A75" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="C75" s="26" t="s">
+      <c r="B75" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="D75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="76" ht="36" customHeight="1" spans="1:4">
-      <c r="A76" s="27" t="s">
+      <c r="C75" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="B76" s="8" t="s">
+    </row>
+    <row r="76" ht="36" customHeight="1" spans="1:3">
+      <c r="A76" s="24" t="s">
         <v>196</v>
       </c>
-      <c r="C76" s="8" t="s">
+      <c r="B76" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="D76" t="s">
-        <v>180</v>
+      <c r="C76" s="28" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="77" ht="63" customHeight="1" spans="1:4">
       <c r="A77" s="20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D77" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" ht="150" spans="1:4">
       <c r="A78" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="C78" s="28" t="s">
         <v>203</v>
       </c>
+      <c r="C78" s="29" t="s">
+        <v>204</v>
+      </c>
       <c r="D78" s="16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" ht="30" spans="1:1">
       <c r="A79" s="20" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" ht="45" spans="1:1">
       <c r="A80" s="20" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" ht="45" spans="1:1">
       <c r="A81" s="20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>